<commit_message>
small update to zoo file
</commit_message>
<xml_diff>
--- a/zoo.xlsx
+++ b/zoo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/colbywitherupwood/Documents/workshops/pythonBootcampFriday/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/colbywitherupwood/Documents/workshops/pandasBasics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7DE4C94-2556-7240-8A75-11F15CC8DAB1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{178B4872-90F8-354F-AD31-1F7D4B283E02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14520" activeTab="1" xr2:uid="{1D7E30CA-E809-414C-A90D-BC0536A5B567}"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14460" xr2:uid="{1D7E30CA-E809-414C-A90D-BC0536A5B567}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{49CFBA46-D056-E441-890A-6C7B2E27C004}" name="zoo" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/colbywitherupwood/Downloads/zoo.csv" comma="1">
+    <textPr sourceFile="/Users/colbywitherupwood/Downloads/zoo.csv" comma="1">
       <textFields count="18">
         <textField/>
         <textField/>
@@ -450,7 +450,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -810,17 +810,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{780D4BFC-F5C3-794D-8F55-85604B04C02B}">
   <dimension ref="A1:R102"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="18" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="1" customFormat="1">
+    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>100</v>
       </c>
@@ -876,7 +876,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -932,7 +932,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -988,7 +988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1044,7 +1044,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1100,7 +1100,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1156,7 +1156,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1212,7 +1212,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1268,7 +1268,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1324,7 +1324,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1380,7 +1380,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1436,7 +1436,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1492,7 +1492,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1548,7 +1548,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1604,7 +1604,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1660,7 +1660,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1716,7 +1716,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:18">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1772,7 +1772,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:18">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1828,7 +1828,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:18">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1884,7 +1884,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:18">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -1940,7 +1940,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:18">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -1996,7 +1996,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:18">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -2052,7 +2052,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:18">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -2108,7 +2108,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:18">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -2164,7 +2164,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:18">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -2220,7 +2220,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:18">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -2276,7 +2276,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:18">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -2332,7 +2332,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:18">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>25</v>
       </c>
@@ -2388,7 +2388,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:18">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>26</v>
       </c>
@@ -2444,7 +2444,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:18">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>27</v>
       </c>
@@ -2500,7 +2500,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:18">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>28</v>
       </c>
@@ -2556,7 +2556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:18">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>29</v>
       </c>
@@ -2612,7 +2612,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:18">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>30</v>
       </c>
@@ -2668,7 +2668,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:18">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>31</v>
       </c>
@@ -2724,7 +2724,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:18">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>32</v>
       </c>
@@ -2780,7 +2780,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:18">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>33</v>
       </c>
@@ -2836,7 +2836,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:18">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>34</v>
       </c>
@@ -2892,7 +2892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:18">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>35</v>
       </c>
@@ -2948,7 +2948,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:18">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>36</v>
       </c>
@@ -3004,7 +3004,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:18">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>37</v>
       </c>
@@ -3060,7 +3060,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:18">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>38</v>
       </c>
@@ -3116,7 +3116,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:18">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>39</v>
       </c>
@@ -3172,7 +3172,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:18">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>40</v>
       </c>
@@ -3228,7 +3228,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:18">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>41</v>
       </c>
@@ -3284,7 +3284,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:18">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>42</v>
       </c>
@@ -3340,7 +3340,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:18">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>43</v>
       </c>
@@ -3396,7 +3396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:18">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>44</v>
       </c>
@@ -3452,7 +3452,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:18">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>45</v>
       </c>
@@ -3508,7 +3508,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:18">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>46</v>
       </c>
@@ -3564,7 +3564,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:18">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>47</v>
       </c>
@@ -3620,7 +3620,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:18">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>48</v>
       </c>
@@ -3676,7 +3676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:18">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>49</v>
       </c>
@@ -3732,7 +3732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:18">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>50</v>
       </c>
@@ -3788,7 +3788,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="54" spans="1:18">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>51</v>
       </c>
@@ -3844,7 +3844,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:18">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>52</v>
       </c>
@@ -3900,7 +3900,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="1:18">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>53</v>
       </c>
@@ -3956,7 +3956,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:18">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>54</v>
       </c>
@@ -4012,7 +4012,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:18">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>55</v>
       </c>
@@ -4068,7 +4068,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:18">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>56</v>
       </c>
@@ -4124,7 +4124,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:18">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>57</v>
       </c>
@@ -4180,7 +4180,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:18">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>58</v>
       </c>
@@ -4236,7 +4236,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:18">
+    <row r="62" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>59</v>
       </c>
@@ -4292,7 +4292,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="1:18">
+    <row r="63" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>60</v>
       </c>
@@ -4348,7 +4348,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:18">
+    <row r="64" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>61</v>
       </c>
@@ -4404,7 +4404,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:18">
+    <row r="65" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>62</v>
       </c>
@@ -4460,7 +4460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:18">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>63</v>
       </c>
@@ -4516,7 +4516,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:18">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>64</v>
       </c>
@@ -4572,7 +4572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:18">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>65</v>
       </c>
@@ -4628,7 +4628,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:18">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>66</v>
       </c>
@@ -4684,7 +4684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:18">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>67</v>
       </c>
@@ -4740,7 +4740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:18">
+    <row r="71" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>68</v>
       </c>
@@ -4796,7 +4796,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:18">
+    <row r="72" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>69</v>
       </c>
@@ -4852,7 +4852,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:18">
+    <row r="73" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>70</v>
       </c>
@@ -4908,7 +4908,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="1:18">
+    <row r="74" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>71</v>
       </c>
@@ -4964,7 +4964,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="75" spans="1:18">
+    <row r="75" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>72</v>
       </c>
@@ -5020,7 +5020,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="76" spans="1:18">
+    <row r="76" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>73</v>
       </c>
@@ -5076,7 +5076,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:18">
+    <row r="77" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>74</v>
       </c>
@@ -5132,7 +5132,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:18">
+    <row r="78" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>75</v>
       </c>
@@ -5188,7 +5188,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="79" spans="1:18">
+    <row r="79" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>76</v>
       </c>
@@ -5244,7 +5244,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="80" spans="1:18">
+    <row r="80" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>77</v>
       </c>
@@ -5300,7 +5300,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="81" spans="1:18">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>78</v>
       </c>
@@ -5356,7 +5356,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="82" spans="1:18">
+    <row r="82" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>79</v>
       </c>
@@ -5412,7 +5412,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="83" spans="1:18">
+    <row r="83" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>80</v>
       </c>
@@ -5468,7 +5468,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="84" spans="1:18">
+    <row r="84" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>81</v>
       </c>
@@ -5524,7 +5524,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="85" spans="1:18">
+    <row r="85" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>82</v>
       </c>
@@ -5580,7 +5580,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="86" spans="1:18">
+    <row r="86" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>83</v>
       </c>
@@ -5636,7 +5636,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:18">
+    <row r="87" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>84</v>
       </c>
@@ -5692,7 +5692,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="88" spans="1:18">
+    <row r="88" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>85</v>
       </c>
@@ -5748,7 +5748,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="89" spans="1:18">
+    <row r="89" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>86</v>
       </c>
@@ -5804,7 +5804,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="90" spans="1:18">
+    <row r="90" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>87</v>
       </c>
@@ -5860,7 +5860,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="91" spans="1:18">
+    <row r="91" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>88</v>
       </c>
@@ -5916,7 +5916,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="92" spans="1:18">
+    <row r="92" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>89</v>
       </c>
@@ -5972,7 +5972,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="93" spans="1:18">
+    <row r="93" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>90</v>
       </c>
@@ -6028,7 +6028,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="94" spans="1:18">
+    <row r="94" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>91</v>
       </c>
@@ -6084,7 +6084,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="95" spans="1:18">
+    <row r="95" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>92</v>
       </c>
@@ -6140,7 +6140,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:18">
+    <row r="96" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>93</v>
       </c>
@@ -6196,7 +6196,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:18">
+    <row r="97" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>94</v>
       </c>
@@ -6252,7 +6252,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="98" spans="1:18">
+    <row r="98" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>95</v>
       </c>
@@ -6308,7 +6308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:18">
+    <row r="99" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>96</v>
       </c>
@@ -6364,7 +6364,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="100" spans="1:18">
+    <row r="100" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>97</v>
       </c>
@@ -6420,7 +6420,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:18">
+    <row r="101" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>98</v>
       </c>
@@ -6476,7 +6476,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="102" spans="1:18">
+    <row r="102" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>99</v>
       </c>
@@ -6541,18 +6541,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1255E2D1-EE41-1140-B8CB-9353F208B102}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -6560,7 +6558,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -6568,7 +6566,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -6576,7 +6574,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -6584,7 +6582,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -6592,7 +6590,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -6600,7 +6598,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>

</xml_diff>